<commit_message>
edit for delete idea
</commit_message>
<xml_diff>
--- a/db/excel/sqlite-inovation-manager-v1.xlsx
+++ b/db/excel/sqlite-inovation-manager-v1.xlsx
@@ -23,7 +23,7 @@
     <sheet name="ideas_questions" sheetId="22" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tables!$A$1:$E$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tables!$A$1:$E$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">users!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="145621" iterateDelta="1E-4" concurrentCalc="0"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="362">
   <si>
     <t>table_name</t>
   </si>
@@ -810,9 +810,6 @@
   </si>
   <si>
     <t>file_path</t>
-  </si>
-  <si>
-    <t>Mã user thực hiện tạo file này</t>
   </si>
   <si>
     <t>Tên file mô tả đầy đủ, chi tiết</t>
@@ -2479,10 +2476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMI68"/>
+  <dimension ref="A1:AMI67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.25"/>
@@ -3541,10 +3538,10 @@
         <v>46</v>
       </c>
       <c r="D2" s="59" t="s">
+        <v>270</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>271</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:1023" ht="37.5">
@@ -3558,7 +3555,7 @@
         <v>240</v>
       </c>
       <c r="D3" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E3" s="26"/>
     </row>
@@ -3573,7 +3570,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E4" s="26"/>
     </row>
@@ -3588,7 +3585,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E5" s="24"/>
     </row>
@@ -3603,7 +3600,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E6" s="24"/>
     </row>
@@ -3618,7 +3615,7 @@
         <v>55</v>
       </c>
       <c r="D7" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E7" s="24"/>
     </row>
@@ -3633,7 +3630,7 @@
         <v>57</v>
       </c>
       <c r="D8" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E8" s="24"/>
     </row>
@@ -3642,13 +3639,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="C9" s="46" t="s">
         <v>273</v>
       </c>
-      <c r="C9" s="46" t="s">
-        <v>274</v>
-      </c>
       <c r="D9" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E9" s="24"/>
     </row>
@@ -3663,7 +3660,7 @@
         <v>237</v>
       </c>
       <c r="D10" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E10" s="24"/>
     </row>
@@ -3678,7 +3675,7 @@
         <v>238</v>
       </c>
       <c r="D11" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E11" s="24"/>
     </row>
@@ -3690,10 +3687,10 @@
         <v>60</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D12" s="62" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>30</v>
@@ -3710,7 +3707,7 @@
         <v>34</v>
       </c>
       <c r="D13" s="60" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E13" s="13"/>
     </row>
@@ -3725,7 +3722,7 @@
         <v>35</v>
       </c>
       <c r="D14" s="60" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E14" s="13"/>
     </row>
@@ -3740,7 +3737,7 @@
         <v>62</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E15" s="58"/>
     </row>
@@ -3755,10 +3752,10 @@
         <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>271</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3772,7 +3769,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E17" s="4"/>
     </row>
@@ -3785,7 +3782,7 @@
       </c>
       <c r="C18" s="50"/>
       <c r="D18" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E18" s="4"/>
     </row>
@@ -3800,7 +3797,7 @@
         <v>249</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E19" s="4"/>
     </row>
@@ -3815,7 +3812,7 @@
         <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E20" s="5"/>
     </row>
@@ -3830,7 +3827,7 @@
         <v>24</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E21" s="6"/>
     </row>
@@ -3845,7 +3842,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E22" s="5"/>
     </row>
@@ -3854,13 +3851,13 @@
         <v>18</v>
       </c>
       <c r="B23" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="C23" s="46" t="s">
         <v>282</v>
       </c>
-      <c r="C23" s="46" t="s">
-        <v>283</v>
-      </c>
       <c r="D23" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E23" s="5"/>
     </row>
@@ -3875,7 +3872,7 @@
         <v>23</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E24" s="5"/>
     </row>
@@ -3887,10 +3884,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E25" s="5"/>
     </row>
@@ -3899,13 +3896,13 @@
         <v>18</v>
       </c>
       <c r="B26" s="31" t="s">
+        <v>293</v>
+      </c>
+      <c r="C26" s="46" t="s">
         <v>294</v>
       </c>
-      <c r="C26" s="46" t="s">
-        <v>295</v>
-      </c>
       <c r="D26" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E26" s="5"/>
     </row>
@@ -3918,10 +3915,10 @@
       </c>
       <c r="C27" s="46"/>
       <c r="D27" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -3929,16 +3926,16 @@
         <v>18</v>
       </c>
       <c r="B28" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="C28" s="46" t="s">
         <v>260</v>
       </c>
-      <c r="C28" s="46" t="s">
-        <v>261</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -3946,16 +3943,16 @@
         <v>18</v>
       </c>
       <c r="B29" s="72" t="s">
+        <v>321</v>
+      </c>
+      <c r="C29" s="49" t="s">
         <v>322</v>
       </c>
-      <c r="C29" s="49" t="s">
-        <v>323</v>
-      </c>
       <c r="D29" s="73" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E29" s="74" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3967,7 +3964,7 @@
       </c>
       <c r="C30" s="46"/>
       <c r="D30" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E30" s="9"/>
     </row>
@@ -3982,10 +3979,10 @@
         <v>232</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E31" s="11" t="s">
         <v>271</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="38.25">
@@ -3999,7 +3996,7 @@
         <v>236</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E32" s="5"/>
     </row>
@@ -4014,7 +4011,7 @@
         <v>250</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E33" s="5"/>
     </row>
@@ -4029,7 +4026,7 @@
         <v>249</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E34" s="4"/>
     </row>
@@ -4038,13 +4035,13 @@
         <v>231</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C35" s="46" t="s">
         <v>234</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E35" s="5"/>
     </row>
@@ -4059,7 +4056,7 @@
         <v>235</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E36" s="5"/>
     </row>
@@ -4074,7 +4071,7 @@
         <v>244</v>
       </c>
       <c r="D37" s="64" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -4083,13 +4080,13 @@
         <v>241</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C38" s="51" t="s">
         <v>242</v>
       </c>
       <c r="D38" s="64" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E38" s="5"/>
     </row>
@@ -4104,7 +4101,7 @@
         <v>245</v>
       </c>
       <c r="D39" s="64" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E39" s="5"/>
     </row>
@@ -4119,7 +4116,7 @@
         <v>246</v>
       </c>
       <c r="D40" s="64" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E40" s="9"/>
     </row>
@@ -4131,13 +4128,13 @@
         <v>6</v>
       </c>
       <c r="C41" s="52" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D41" s="65" t="s">
+        <v>270</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>271</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -4148,10 +4145,10 @@
         <v>251</v>
       </c>
       <c r="C42" s="46" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D42" s="66" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E42" s="5"/>
     </row>
@@ -4166,7 +4163,7 @@
         <v>252</v>
       </c>
       <c r="D43" s="65" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E43" s="5"/>
     </row>
@@ -4181,7 +4178,7 @@
         <v>253</v>
       </c>
       <c r="D44" s="65" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E44" s="5"/>
     </row>
@@ -4193,10 +4190,10 @@
         <v>256</v>
       </c>
       <c r="C45" s="46" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D45" s="66" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E45" s="5"/>
     </row>
@@ -4211,66 +4208,66 @@
         <v>245</v>
       </c>
       <c r="D46" s="64" t="s">
+        <v>270</v>
+      </c>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="43" t="s">
+        <v>261</v>
+      </c>
+      <c r="B47" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="D47" s="67" t="s">
+        <v>270</v>
+      </c>
+      <c r="E47" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="44" t="s">
-        <v>247</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C47" s="46" t="s">
-        <v>257</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E47" s="9"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B48" s="37" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C48" s="46" t="s">
         <v>263</v>
       </c>
       <c r="D48" s="67" t="s">
-        <v>271</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>272</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="43" t="s">
-        <v>262</v>
-      </c>
-      <c r="B49" s="37" t="s">
-        <v>25</v>
+        <v>261</v>
+      </c>
+      <c r="B49" s="33" t="s">
+        <v>59</v>
       </c>
       <c r="C49" s="46" t="s">
-        <v>264</v>
+        <v>297</v>
       </c>
       <c r="D49" s="67" t="s">
-        <v>270</v>
-      </c>
-      <c r="E49" s="5"/>
+        <v>269</v>
+      </c>
+      <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" s="46" t="s">
-        <v>298</v>
+        <v>337</v>
+      </c>
+      <c r="C50" s="81" t="s">
+        <v>338</v>
       </c>
       <c r="D50" s="67" t="s">
         <v>270</v>
@@ -4279,129 +4276,129 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="43" t="s">
-        <v>262</v>
-      </c>
-      <c r="B51" s="33" t="s">
-        <v>338</v>
-      </c>
-      <c r="C51" s="81" t="s">
-        <v>339</v>
+        <v>261</v>
+      </c>
+      <c r="B51" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="46" t="s">
+        <v>274</v>
       </c>
       <c r="D51" s="67" t="s">
-        <v>271</v>
-      </c>
-      <c r="E51" s="1"/>
+        <v>270</v>
+      </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="43" t="s">
-        <v>262</v>
-      </c>
-      <c r="B52" s="37" t="s">
-        <v>5</v>
+      <c r="A52" s="55" t="s">
+        <v>264</v>
+      </c>
+      <c r="B52" s="76" t="s">
+        <v>6</v>
       </c>
       <c r="C52" s="46" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="D52" s="67" t="s">
+        <v>270</v>
+      </c>
+      <c r="E52" s="11" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="55" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B53" s="76" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C53" s="46" t="s">
         <v>266</v>
       </c>
       <c r="D53" s="67" t="s">
-        <v>271</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>272</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="E53" s="5"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="55" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B54" s="76" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="46" t="s">
-        <v>267</v>
+        <v>337</v>
+      </c>
+      <c r="C54" s="81" t="s">
+        <v>338</v>
       </c>
       <c r="D54" s="67" t="s">
         <v>270</v>
       </c>
-      <c r="E54" s="5"/>
+      <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="55" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B55" s="76" t="s">
-        <v>338</v>
-      </c>
-      <c r="C55" s="81" t="s">
-        <v>339</v>
+        <v>5</v>
+      </c>
+      <c r="C55" s="46" t="s">
+        <v>274</v>
       </c>
       <c r="D55" s="67" t="s">
-        <v>271</v>
-      </c>
-      <c r="E55" s="1"/>
+        <v>270</v>
+      </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="55" t="s">
-        <v>265</v>
-      </c>
-      <c r="B56" s="76" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="46" t="s">
-        <v>275</v>
-      </c>
-      <c r="D56" s="67" t="s">
+      <c r="A56" s="71" t="s">
+        <v>307</v>
+      </c>
+      <c r="B56" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="49" t="s">
+        <v>308</v>
+      </c>
+      <c r="D56" s="69" t="s">
+        <v>270</v>
+      </c>
+      <c r="E56" s="11" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="71" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B57" s="72" t="s">
-        <v>6</v>
+        <v>320</v>
       </c>
       <c r="C57" s="49" t="s">
         <v>309</v>
       </c>
       <c r="D57" s="69" t="s">
-        <v>271</v>
-      </c>
-      <c r="E57" s="11" t="s">
-        <v>272</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="71" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B58" s="72" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="C58" s="49" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D58" s="69" t="s">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="E58" s="5"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="71" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B59" s="72" t="s">
         <v>312</v>
@@ -4410,149 +4407,134 @@
         <v>314</v>
       </c>
       <c r="D59" s="69" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E59" s="5"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="71" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B60" s="72" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C60" s="49" t="s">
+        <v>317</v>
+      </c>
+      <c r="D60" s="69" t="s">
         <v>315</v>
       </c>
-      <c r="D60" s="69" t="s">
-        <v>316</v>
-      </c>
       <c r="E60" s="5"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" ht="38.25">
       <c r="A61" s="71" t="s">
-        <v>308</v>
-      </c>
-      <c r="B61" s="72" t="s">
-        <v>317</v>
+        <v>307</v>
+      </c>
+      <c r="B61" s="70" t="s">
+        <v>5</v>
       </c>
       <c r="C61" s="49" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="D61" s="69" t="s">
-        <v>316</v>
+        <v>270</v>
       </c>
       <c r="E61" s="5"/>
     </row>
-    <row r="62" spans="1:5" ht="38.25">
-      <c r="A62" s="71" t="s">
-        <v>308</v>
-      </c>
-      <c r="B62" s="70" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="49" t="s">
-        <v>324</v>
-      </c>
-      <c r="D62" s="69" t="s">
-        <v>271</v>
-      </c>
-      <c r="E62" s="5"/>
-    </row>
-    <row r="63" spans="1:5">
+    <row r="62" spans="1:5">
+      <c r="A62" s="55" t="s">
+        <v>306</v>
+      </c>
+      <c r="B62" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="C62" s="81" t="s">
+        <v>356</v>
+      </c>
+      <c r="D62" s="67" t="s">
+        <v>270</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="38.25">
       <c r="A63" s="55" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B63" s="31" t="s">
-        <v>293</v>
+        <v>310</v>
       </c>
       <c r="C63" s="81" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D63" s="67" t="s">
-        <v>271</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>336</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:5" ht="38.25">
       <c r="A64" s="55" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B64" s="31" t="s">
-        <v>311</v>
+        <v>13</v>
       </c>
       <c r="C64" s="81" t="s">
         <v>355</v>
       </c>
       <c r="D64" s="67" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E64" s="5"/>
     </row>
-    <row r="65" spans="1:5" ht="38.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="55" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B65" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C65" s="81" t="s">
-        <v>356</v>
-      </c>
-      <c r="D65" s="67" t="s">
-        <v>271</v>
+        <v>318</v>
+      </c>
+      <c r="C65" s="46" t="s">
+        <v>319</v>
+      </c>
+      <c r="D65" s="69" t="s">
+        <v>315</v>
       </c>
       <c r="E65" s="5"/>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="55" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B66" s="31" t="s">
-        <v>319</v>
-      </c>
-      <c r="C66" s="46" t="s">
-        <v>320</v>
+        <v>14</v>
+      </c>
+      <c r="C66" s="49" t="s">
+        <v>34</v>
       </c>
       <c r="D66" s="69" t="s">
-        <v>316</v>
+        <v>270</v>
       </c>
       <c r="E66" s="5"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="55" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B67" s="31" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C67" s="49" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="D67" s="69" t="s">
-        <v>271</v>
-      </c>
-      <c r="E67" s="5"/>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="55" t="s">
-        <v>307</v>
-      </c>
-      <c r="B68" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C68" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="D68" s="69" t="s">
-        <v>271</v>
-      </c>
-      <c r="E68" s="9"/>
+        <v>270</v>
+      </c>
+      <c r="E67" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E56"/>
+  <autoFilter ref="A1:E55"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
@@ -4699,7 +4681,7 @@
         <v>56</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I1" s="25" t="s">
         <v>58</v>
@@ -4725,31 +4707,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C2">
         <v>123</v>
       </c>
       <c r="D2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F2" s="77" t="s">
+        <v>334</v>
+      </c>
+      <c r="G2" t="s">
         <v>331</v>
       </c>
-      <c r="E2" t="s">
-        <v>333</v>
-      </c>
-      <c r="F2" s="77" t="s">
-        <v>335</v>
-      </c>
-      <c r="G2" t="s">
-        <v>332</v>
-      </c>
       <c r="H2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -4769,31 +4751,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C3">
         <v>123</v>
       </c>
       <c r="D3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E3" t="s">
+        <v>333</v>
+      </c>
+      <c r="F3" s="77" t="s">
+        <v>334</v>
+      </c>
+      <c r="G3" t="s">
         <v>331</v>
       </c>
-      <c r="E3" t="s">
-        <v>334</v>
-      </c>
-      <c r="F3" s="77" t="s">
-        <v>335</v>
-      </c>
-      <c r="G3" t="s">
-        <v>332</v>
-      </c>
       <c r="H3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K3">
         <v>99</v>
@@ -4813,31 +4795,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C4">
         <v>123</v>
       </c>
       <c r="D4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E4" t="s">
+        <v>341</v>
+      </c>
+      <c r="F4" s="77" t="s">
+        <v>334</v>
+      </c>
+      <c r="G4" t="s">
         <v>331</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
+        <v>336</v>
+      </c>
+      <c r="I4" t="s">
         <v>342</v>
       </c>
-      <c r="F4" s="77" t="s">
-        <v>335</v>
-      </c>
-      <c r="G4" t="s">
-        <v>332</v>
-      </c>
-      <c r="H4" t="s">
-        <v>337</v>
-      </c>
-      <c r="I4" t="s">
-        <v>343</v>
-      </c>
       <c r="J4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -4897,7 +4879,7 @@
         <v>59</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>5</v>
@@ -4908,10 +4890,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5">
@@ -4923,10 +4905,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
@@ -4940,10 +4922,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5">
@@ -4955,10 +4937,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5">
@@ -4970,10 +4952,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5">
@@ -4985,10 +4967,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5">
@@ -5000,10 +4982,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5">
@@ -5015,10 +4997,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5">
@@ -5060,7 +5042,7 @@
         <v>25</v>
       </c>
       <c r="C1" s="80" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D1" s="76" t="s">
         <v>5</v>
@@ -5071,7 +5053,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5">
@@ -5083,7 +5065,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -5097,7 +5079,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5">
@@ -5109,7 +5091,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5">
@@ -5121,7 +5103,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5">
@@ -5133,7 +5115,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5">
@@ -5180,16 +5162,16 @@
         <v>6</v>
       </c>
       <c r="B1" s="72" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" s="72" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1" s="72" t="s">
         <v>312</v>
       </c>
-      <c r="D1" s="72" t="s">
-        <v>313</v>
-      </c>
       <c r="E1" s="72" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F1" s="70" t="s">
         <v>5</v>
@@ -5200,7 +5182,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -5220,7 +5202,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -5240,7 +5222,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -5260,7 +5242,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -5280,7 +5262,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -5346,7 +5328,7 @@
         <v>14</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I1" s="31" t="s">
         <v>15</v>
@@ -5355,16 +5337,16 @@
         <v>17</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L1" s="31" t="s">
         <v>16</v>
       </c>
       <c r="M1" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N1" s="72" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O1" s="75" t="s">
         <v>11</v>
@@ -5375,10 +5357,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C2" t="s">
         <v>344</v>
-      </c>
-      <c r="C2" t="s">
-        <v>345</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -5390,7 +5372,7 @@
         <v>1590045283916</v>
       </c>
       <c r="H2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -5410,10 +5392,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C3" t="s">
         <v>346</v>
-      </c>
-      <c r="C3" t="s">
-        <v>347</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -5425,7 +5407,7 @@
         <v>1590045323073</v>
       </c>
       <c r="H3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -5445,10 +5427,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -5460,7 +5442,7 @@
         <v>1590045603862</v>
       </c>
       <c r="H4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -5480,10 +5462,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C5" t="s">
         <v>348</v>
-      </c>
-      <c r="C5" t="s">
-        <v>349</v>
       </c>
       <c r="E5">
         <v>7</v>
@@ -5495,7 +5477,7 @@
         <v>1590045634319</v>
       </c>
       <c r="H5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -5515,10 +5497,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" t="s">
         <v>351</v>
-      </c>
-      <c r="C6" t="s">
-        <v>352</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -5530,7 +5512,7 @@
         <v>1590047016939</v>
       </c>
       <c r="H6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -5550,10 +5532,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C7" t="s">
         <v>353</v>
-      </c>
-      <c r="C7" t="s">
-        <v>354</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -5565,7 +5547,7 @@
         <v>1590047072983</v>
       </c>
       <c r="H7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -5757,7 +5739,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>36</v>
@@ -6886,10 +6868,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
+        <v>275</v>
+      </c>
+      <c r="H2" t="s">
         <v>276</v>
-      </c>
-      <c r="H2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -6900,10 +6882,10 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
+        <v>277</v>
+      </c>
+      <c r="H3" t="s">
         <v>278</v>
-      </c>
-      <c r="H3" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit excel to db
</commit_message>
<xml_diff>
--- a/db/excel/sqlite-inovation-manager-v1.xlsx
+++ b/db/excel/sqlite-inovation-manager-v1.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DINHNV\MyData\LAPTRINH\NODE4\node4-inovation\db\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF19C25-0B3C-4300-B42B-D5F35876C2AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -45,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="359">
   <si>
     <t>table_name</t>
   </si>
@@ -248,9 +242,6 @@
     <t>change_time</t>
   </si>
   <si>
-    <t>Thời gian thay đổi tham số</t>
-  </si>
-  <si>
     <t>delete_logentry</t>
   </si>
   <si>
@@ -914,9 +905,6 @@
     <t>burlywood</t>
   </si>
   <si>
-    <t>ideas_marks</t>
-  </si>
-  <si>
     <t>ideas_questions</t>
   </si>
   <si>
@@ -926,9 +914,6 @@
     <t>Câu hỏi gì để cho điểm</t>
   </si>
   <si>
-    <t>question_id</t>
-  </si>
-  <si>
     <t>min_point</t>
   </si>
   <si>
@@ -950,12 +935,6 @@
     <t>trọng số đánh giá này</t>
   </si>
   <si>
-    <t>point</t>
-  </si>
-  <si>
-    <t>cho mấy điểm</t>
-  </si>
-  <si>
     <t>question</t>
   </si>
   <si>
@@ -1055,48 +1034,6 @@
     <t>Mô tả Ý tưởng thứ hai của dinh99</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">câu hỏi nào </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(nhớ tạo PRIMARY KEY sau khi tạo đc csdl)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">user nào, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(nhớ tạo PRIMARY KEY sau khi tạo đc csdl)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ý tưởng nào </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(tạo PRIMARY KEY khi tạo csdl)</t>
-    </r>
-  </si>
-  <si>
     <t>Mô tả Ý tưởng đầu tiên của dinh1</t>
   </si>
   <si>
@@ -1110,9 +1047,6 @@
   </si>
   <si>
     <t>Có thể triển khai sau</t>
-  </si>
-  <si>
-    <t>, FOREIGN KEY (idea_id) REFERENCES ideas(id), FOREIGN KEY (question_id) REFERENCES ideas_questions(id), FOREIGN KEY (user_id) REFERENCES users(id)</t>
   </si>
   <si>
     <t>,  FOREIGN KEY (category_id) REFERENCES ideas_categories(id),  FOREIGN KEY (user_id) REFERENCES users(id),  FOREIGN KEY (status) REFERENCES ideas_statuses(id)</t>
@@ -1187,11 +1121,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1314,12 +1248,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1401,7 +1329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="28">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1512,12 +1440,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
@@ -1790,7 +1712,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1904,108 +1826,95 @@
     <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2597,11 +2506,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMI68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMI62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:XFD63"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="23.25"/>
@@ -3657,13 +3566,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="D2" s="47" t="s">
+        <v>255</v>
+      </c>
+      <c r="E2" s="41" t="s">
         <v>256</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:1023">
@@ -3674,10 +3583,10 @@
         <v>45</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E3" s="41"/>
     </row>
@@ -3686,13 +3595,13 @@
         <v>43</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E4" s="41"/>
     </row>
@@ -3704,10 +3613,10 @@
         <v>46</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E5" s="41"/>
     </row>
@@ -3719,10 +3628,10 @@
         <v>47</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E6" s="41"/>
     </row>
@@ -3737,7 +3646,7 @@
         <v>49</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E7" s="41"/>
     </row>
@@ -3752,7 +3661,7 @@
         <v>51</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E8" s="41"/>
     </row>
@@ -3761,13 +3670,13 @@
         <v>43</v>
       </c>
       <c r="B9" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="C9" s="39" t="s">
         <v>258</v>
       </c>
-      <c r="C9" s="39" t="s">
-        <v>259</v>
-      </c>
       <c r="D9" s="40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E9" s="41"/>
     </row>
@@ -3779,10 +3688,10 @@
         <v>52</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E10" s="41"/>
     </row>
@@ -3794,10 +3703,10 @@
         <v>53</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E11" s="41"/>
     </row>
@@ -3809,10 +3718,10 @@
         <v>54</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E12" s="41" t="s">
         <v>28</v>
@@ -3829,7 +3738,7 @@
         <v>32</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E13" s="43"/>
     </row>
@@ -3844,7 +3753,7 @@
         <v>33</v>
       </c>
       <c r="D14" s="42" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E14" s="43"/>
     </row>
@@ -3856,10 +3765,10 @@
         <v>11</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E15" s="45"/>
     </row>
@@ -3874,10 +3783,10 @@
         <v>19</v>
       </c>
       <c r="D16" s="55" t="s">
+        <v>255</v>
+      </c>
+      <c r="E16" s="56" t="s">
         <v>256</v>
-      </c>
-      <c r="E16" s="56" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3891,7 +3800,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="55" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E17" s="55"/>
     </row>
@@ -3903,10 +3812,10 @@
         <v>2</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="D18" s="55" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E18" s="55"/>
     </row>
@@ -3915,13 +3824,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="53" t="s">
+        <v>235</v>
+      </c>
+      <c r="C19" s="54" t="s">
         <v>236</v>
       </c>
-      <c r="C19" s="54" t="s">
-        <v>237</v>
-      </c>
       <c r="D19" s="55" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E19" s="55"/>
     </row>
@@ -3936,7 +3845,7 @@
         <v>21</v>
       </c>
       <c r="D20" s="55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E20" s="59"/>
     </row>
@@ -3951,7 +3860,7 @@
         <v>22</v>
       </c>
       <c r="D21" s="55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E21" s="59"/>
     </row>
@@ -3963,10 +3872,10 @@
         <v>14</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="D22" s="55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E22" s="59"/>
     </row>
@@ -3975,13 +3884,13 @@
         <v>18</v>
       </c>
       <c r="B23" s="53" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="D23" s="55" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E23" s="59"/>
     </row>
@@ -3993,10 +3902,10 @@
         <v>15</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="D24" s="55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E24" s="59"/>
     </row>
@@ -4008,10 +3917,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D25" s="55" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E25" s="59"/>
     </row>
@@ -4020,13 +3929,13 @@
         <v>18</v>
       </c>
       <c r="B26" s="53" t="s">
+        <v>277</v>
+      </c>
+      <c r="C26" s="58" t="s">
         <v>278</v>
       </c>
-      <c r="C26" s="58" t="s">
-        <v>279</v>
-      </c>
       <c r="D26" s="55" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E26" s="59"/>
     </row>
@@ -4038,13 +3947,13 @@
         <v>16</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="D27" s="55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E27" s="59" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -4052,16 +3961,16 @@
         <v>18</v>
       </c>
       <c r="B28" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="C28" s="58" t="s">
         <v>245</v>
       </c>
-      <c r="C28" s="58" t="s">
-        <v>246</v>
-      </c>
       <c r="D28" s="55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E28" s="59" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -4069,16 +3978,16 @@
         <v>18</v>
       </c>
       <c r="B29" s="53" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D29" s="55" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E29" s="59" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="74.25" customHeight="1">
@@ -4089,605 +3998,513 @@
         <v>11</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="D30" s="55" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E30" s="60" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="61" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B31" s="62" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D31" s="50" t="s">
+        <v>255</v>
+      </c>
+      <c r="E31" s="63" t="s">
         <v>256</v>
-      </c>
-      <c r="E31" s="63" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="61" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B32" s="62" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D32" s="50" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E32" s="51"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="61" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B33" s="62" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="D33" s="50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E33" s="51"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="61" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B34" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="C34" s="64" t="s">
         <v>236</v>
       </c>
-      <c r="C34" s="64" t="s">
-        <v>237</v>
-      </c>
       <c r="D34" s="50" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E34" s="50"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="61" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B35" s="62" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C35" s="49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D35" s="50" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E35" s="51"/>
     </row>
     <row r="36" spans="1:5" ht="31.5">
       <c r="A36" s="61" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B36" s="62" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="49" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D36" s="50" t="s">
-        <v>256</v>
-      </c>
-      <c r="E36" s="103" t="s">
-        <v>366</v>
+        <v>255</v>
+      </c>
+      <c r="E36" s="96" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B37" s="72" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="72" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="D37" s="72" t="s">
+        <v>255</v>
+      </c>
+      <c r="E37" s="72" t="s">
         <v>256</v>
-      </c>
-      <c r="E37" s="72" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B38" s="71" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="72" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D38" s="73" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E38" s="74"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="70" t="s">
+        <v>229</v>
+      </c>
+      <c r="B39" s="75" t="s">
+        <v>276</v>
+      </c>
+      <c r="C39" s="72" t="s">
         <v>230</v>
       </c>
-      <c r="B39" s="75" t="s">
-        <v>277</v>
-      </c>
-      <c r="C39" s="72" t="s">
-        <v>231</v>
-      </c>
       <c r="D39" s="73" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E39" s="74"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B40" s="71" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="72" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="D40" s="73" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E40" s="74"/>
     </row>
     <row r="41" spans="1:5" ht="31.5">
       <c r="A41" s="70" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B41" s="71" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C41" s="72" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D41" s="73" t="s">
-        <v>256</v>
-      </c>
-      <c r="E41" s="104" t="s">
-        <v>366</v>
+        <v>255</v>
+      </c>
+      <c r="E41" s="97" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="65" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B42" s="66" t="s">
         <v>6</v>
       </c>
       <c r="C42" s="67" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="D42" s="68" t="s">
+        <v>255</v>
+      </c>
+      <c r="E42" s="76" t="s">
         <v>256</v>
-      </c>
-      <c r="E42" s="76" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="65" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B43" s="66" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C43" s="67" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D43" s="77" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E43" s="69"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="65" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B44" s="66" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C44" s="67" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D44" s="68" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E44" s="69"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="65" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B45" s="66" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C45" s="67" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D45" s="68" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E45" s="69"/>
     </row>
     <row r="46" spans="1:5" ht="38.25">
       <c r="A46" s="65" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B46" s="66" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C46" s="67" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="D46" s="77" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E46" s="69"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="65" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B47" s="66" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="67" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="D47" s="68" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E47" s="69"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="78" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B48" s="53" t="s">
         <v>6</v>
       </c>
       <c r="C48" s="58" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D48" s="79" t="s">
+        <v>255</v>
+      </c>
+      <c r="E48" s="56" t="s">
         <v>256</v>
-      </c>
-      <c r="E48" s="56" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="78" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B49" s="53" t="s">
         <v>23</v>
       </c>
       <c r="C49" s="58" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D49" s="79" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E49" s="59"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="78" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B50" s="53" t="s">
         <v>53</v>
       </c>
       <c r="C50" s="58" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D50" s="79" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E50" s="59"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="78" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B51" s="53" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C51" s="58" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D51" s="79" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E51" s="59"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="78" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B52" s="53" t="s">
         <v>5</v>
       </c>
       <c r="C52" s="58" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D52" s="79" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E52" s="59"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="80" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B53" s="81" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="82" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D53" s="83" t="s">
+        <v>255</v>
+      </c>
+      <c r="E53" s="84" t="s">
         <v>256</v>
-      </c>
-      <c r="E53" s="84" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="80" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B54" s="81" t="s">
         <v>23</v>
       </c>
       <c r="C54" s="82" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D54" s="83" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E54" s="85"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="80" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B55" s="81" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C55" s="82" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D55" s="83" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E55" s="85"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="80" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B56" s="81" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="82" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D56" s="83" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E56" s="85"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="86" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B57" s="87" t="s">
         <v>6</v>
       </c>
       <c r="C57" s="88" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D57" s="89" t="s">
+        <v>255</v>
+      </c>
+      <c r="E57" s="90" t="s">
         <v>256</v>
-      </c>
-      <c r="E57" s="90" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="86" t="s">
+        <v>288</v>
+      </c>
+      <c r="B58" s="87" t="s">
+        <v>298</v>
+      </c>
+      <c r="C58" s="88" t="s">
         <v>290</v>
       </c>
-      <c r="B58" s="87" t="s">
-        <v>303</v>
-      </c>
-      <c r="C58" s="88" t="s">
-        <v>292</v>
-      </c>
       <c r="D58" s="89" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E58" s="74"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="86" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B59" s="87" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C59" s="88" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D59" s="89" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E59" s="74"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="86" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B60" s="87" t="s">
+        <v>292</v>
+      </c>
+      <c r="C60" s="88" t="s">
+        <v>294</v>
+      </c>
+      <c r="D60" s="89" t="s">
         <v>295</v>
-      </c>
-      <c r="C60" s="88" t="s">
-        <v>297</v>
-      </c>
-      <c r="D60" s="89" t="s">
-        <v>298</v>
       </c>
       <c r="E60" s="74"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="86" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B61" s="87" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C61" s="88" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D61" s="89" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E61" s="74"/>
     </row>
     <row r="62" spans="1:5" ht="38.25">
       <c r="A62" s="86" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B62" s="91" t="s">
         <v>5</v>
       </c>
       <c r="C62" s="88" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D62" s="89" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E62" s="74"/>
     </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="92" t="s">
-        <v>289</v>
-      </c>
-      <c r="B63" s="93" t="s">
-        <v>277</v>
-      </c>
-      <c r="C63" s="94" t="s">
-        <v>338</v>
-      </c>
-      <c r="D63" s="95" t="s">
-        <v>256</v>
-      </c>
-      <c r="E63" s="96"/>
-    </row>
-    <row r="64" spans="1:5" ht="38.25">
-      <c r="A64" s="92" t="s">
-        <v>289</v>
-      </c>
-      <c r="B64" s="93" t="s">
-        <v>293</v>
-      </c>
-      <c r="C64" s="94" t="s">
-        <v>336</v>
-      </c>
-      <c r="D64" s="95" t="s">
-        <v>256</v>
-      </c>
-      <c r="E64" s="96"/>
-    </row>
-    <row r="65" spans="1:5" ht="38.25">
-      <c r="A65" s="92" t="s">
-        <v>289</v>
-      </c>
-      <c r="B65" s="93" t="s">
-        <v>13</v>
-      </c>
-      <c r="C65" s="94" t="s">
-        <v>337</v>
-      </c>
-      <c r="D65" s="95" t="s">
-        <v>256</v>
-      </c>
-      <c r="E65" s="96"/>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="92" t="s">
-        <v>289</v>
-      </c>
-      <c r="B66" s="93" t="s">
-        <v>301</v>
-      </c>
-      <c r="C66" s="97" t="s">
-        <v>302</v>
-      </c>
-      <c r="D66" s="95" t="s">
-        <v>298</v>
-      </c>
-      <c r="E66" s="96"/>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="92" t="s">
-        <v>289</v>
-      </c>
-      <c r="B67" s="93" t="s">
-        <v>14</v>
-      </c>
-      <c r="C67" s="97" t="s">
-        <v>32</v>
-      </c>
-      <c r="D67" s="95" t="s">
-        <v>256</v>
-      </c>
-      <c r="E67" s="96"/>
-    </row>
-    <row r="68" spans="1:5" ht="61.5" customHeight="1">
-      <c r="A68" s="92" t="s">
-        <v>289</v>
-      </c>
-      <c r="B68" s="93" t="s">
-        <v>42</v>
-      </c>
-      <c r="C68" s="97" t="s">
-        <v>67</v>
-      </c>
-      <c r="D68" s="95" t="s">
-        <v>256</v>
-      </c>
-      <c r="E68" s="98" t="s">
-        <v>344</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E56" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E56"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
@@ -4699,7 +4516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4787,7 +4604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4817,7 +4634,7 @@
         <v>45</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>46</v>
@@ -4832,7 +4649,7 @@
         <v>50</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I1" s="19" t="s">
         <v>52</v>
@@ -4858,31 +4675,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C2">
         <v>123</v>
       </c>
       <c r="D2" t="s">
+        <v>308</v>
+      </c>
+      <c r="E2" t="s">
+        <v>310</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="G2" t="s">
+        <v>309</v>
+      </c>
+      <c r="H2" t="s">
         <v>313</v>
       </c>
-      <c r="E2" t="s">
-        <v>315</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G2" t="s">
-        <v>314</v>
-      </c>
-      <c r="H2" t="s">
-        <v>318</v>
-      </c>
       <c r="I2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J2" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -4902,31 +4719,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C3">
         <v>123</v>
       </c>
       <c r="D3" t="s">
+        <v>308</v>
+      </c>
+      <c r="E3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="G3" t="s">
+        <v>309</v>
+      </c>
+      <c r="H3" t="s">
         <v>313</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>316</v>
       </c>
-      <c r="F3" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G3" t="s">
-        <v>314</v>
-      </c>
-      <c r="H3" t="s">
-        <v>318</v>
-      </c>
-      <c r="I3" t="s">
-        <v>321</v>
-      </c>
       <c r="J3" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="K3">
         <v>99</v>
@@ -4946,31 +4763,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C4">
         <v>123</v>
       </c>
       <c r="D4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E4" t="s">
+        <v>318</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="G4" t="s">
+        <v>309</v>
+      </c>
+      <c r="H4" t="s">
         <v>313</v>
       </c>
-      <c r="E4" t="s">
-        <v>323</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>317</v>
-      </c>
-      <c r="G4" t="s">
-        <v>314</v>
-      </c>
-      <c r="H4" t="s">
-        <v>318</v>
-      </c>
       <c r="I4" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -4986,11 +4803,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
+  <autoFilter ref="A1:N1"/>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -5003,7 +4820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5030,7 +4847,7 @@
         <v>53</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E1" s="24" t="s">
         <v>5</v>
@@ -5041,10 +4858,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4">
@@ -5056,10 +4873,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -5073,10 +4890,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4">
@@ -5088,10 +4905,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4">
@@ -5103,10 +4920,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4">
@@ -5118,10 +4935,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4">
@@ -5133,10 +4950,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
@@ -5148,10 +4965,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4">
@@ -5170,7 +4987,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5193,7 +5010,7 @@
         <v>23</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D1" s="32" t="s">
         <v>5</v>
@@ -5204,7 +5021,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4">
@@ -5216,7 +5033,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
@@ -5230,7 +5047,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4">
@@ -5242,7 +5059,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4">
@@ -5254,7 +5071,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4">
@@ -5266,7 +5083,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4">
@@ -5291,7 +5108,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5313,16 +5130,16 @@
         <v>6</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F1" s="30" t="s">
         <v>5</v>
@@ -5333,7 +5150,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -5353,7 +5170,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -5373,7 +5190,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -5393,7 +5210,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -5413,7 +5230,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -5440,7 +5257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5455,49 +5272,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.75">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="100" t="s">
+      <c r="C1" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="100" t="s">
-        <v>236</v>
-      </c>
-      <c r="E1" s="100" t="s">
+      <c r="D1" s="93" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="101" t="s">
+      <c r="G1" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="100" t="s">
-        <v>267</v>
-      </c>
-      <c r="I1" s="100" t="s">
+      <c r="H1" s="93" t="s">
+        <v>266</v>
+      </c>
+      <c r="I1" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="100" t="s">
+      <c r="J1" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="100" t="s">
-        <v>278</v>
-      </c>
-      <c r="L1" s="100" t="s">
+      <c r="K1" s="93" t="s">
+        <v>277</v>
+      </c>
+      <c r="L1" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="100" t="s">
-        <v>245</v>
-      </c>
-      <c r="N1" s="100" t="s">
-        <v>304</v>
-      </c>
-      <c r="O1" s="102" t="s">
+      <c r="M1" s="93" t="s">
+        <v>244</v>
+      </c>
+      <c r="N1" s="93" t="s">
+        <v>299</v>
+      </c>
+      <c r="O1" s="95" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5506,10 +5323,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C2" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -5521,7 +5338,7 @@
         <v>1590045283916</v>
       </c>
       <c r="H2" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -5541,10 +5358,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C3" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -5556,7 +5373,7 @@
         <v>1590045323073</v>
       </c>
       <c r="H3" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -5576,10 +5393,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>326</v>
+      </c>
+      <c r="C4" t="s">
         <v>331</v>
-      </c>
-      <c r="C4" t="s">
-        <v>339</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -5591,7 +5408,7 @@
         <v>1590045603862</v>
       </c>
       <c r="H4" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -5611,10 +5428,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C5" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="E5">
         <v>7</v>
@@ -5626,7 +5443,7 @@
         <v>1590045634319</v>
       </c>
       <c r="H5" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -5646,10 +5463,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C6" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -5661,7 +5478,7 @@
         <v>1590047016939</v>
       </c>
       <c r="H6" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -5681,10 +5498,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C7" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -5696,7 +5513,7 @@
         <v>1590047072983</v>
       </c>
       <c r="H7" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -5718,7 +5535,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5790,7 +5607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5863,7 +5680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5888,7 +5705,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>34</v>
@@ -5920,13 +5737,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>169</v>
-      </c>
       <c r="E2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -5937,13 +5754,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>171</v>
-      </c>
       <c r="E3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -5954,13 +5771,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>69</v>
-      </c>
       <c r="E4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -5971,13 +5788,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>71</v>
-      </c>
       <c r="E5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -5988,13 +5805,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>73</v>
-      </c>
       <c r="E6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -6005,13 +5822,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>75</v>
-      </c>
       <c r="E7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -6022,13 +5839,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>77</v>
-      </c>
       <c r="E8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -6039,13 +5856,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>79</v>
-      </c>
       <c r="E9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -6056,13 +5873,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>81</v>
-      </c>
       <c r="E10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -6073,13 +5890,13 @@
         <v>3</v>
       </c>
       <c r="C11" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>83</v>
-      </c>
       <c r="E11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -6090,13 +5907,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="23" t="s">
-        <v>85</v>
-      </c>
       <c r="E12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -6107,13 +5924,13 @@
         <v>3</v>
       </c>
       <c r="C13" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>87</v>
-      </c>
       <c r="E13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -6124,13 +5941,13 @@
         <v>4</v>
       </c>
       <c r="C14" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>89</v>
-      </c>
       <c r="E14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -6141,13 +5958,13 @@
         <v>4</v>
       </c>
       <c r="C15" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>91</v>
-      </c>
       <c r="E15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -6158,13 +5975,13 @@
         <v>4</v>
       </c>
       <c r="C16" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>93</v>
-      </c>
       <c r="E16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -6175,13 +5992,13 @@
         <v>4</v>
       </c>
       <c r="C17" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="23" t="s">
-        <v>95</v>
-      </c>
       <c r="E17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6192,13 +6009,13 @@
         <v>5</v>
       </c>
       <c r="C18" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="23" t="s">
-        <v>97</v>
-      </c>
       <c r="E18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -6209,13 +6026,13 @@
         <v>5</v>
       </c>
       <c r="C19" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="23" t="s">
-        <v>99</v>
-      </c>
       <c r="E19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -6226,13 +6043,13 @@
         <v>5</v>
       </c>
       <c r="C20" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>101</v>
-      </c>
       <c r="E20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -6243,13 +6060,13 @@
         <v>5</v>
       </c>
       <c r="C21" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="23" t="s">
-        <v>103</v>
-      </c>
       <c r="E21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -6260,13 +6077,13 @@
         <v>6</v>
       </c>
       <c r="C22" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="23" t="s">
-        <v>105</v>
-      </c>
       <c r="E22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -6277,13 +6094,13 @@
         <v>6</v>
       </c>
       <c r="C23" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="23" t="s">
-        <v>107</v>
-      </c>
       <c r="E23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -6294,13 +6111,13 @@
         <v>6</v>
       </c>
       <c r="C24" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="23" t="s">
-        <v>109</v>
-      </c>
       <c r="E24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -6311,13 +6128,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="D25" s="23" t="s">
-        <v>111</v>
-      </c>
       <c r="E25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -6328,13 +6145,13 @@
         <v>7</v>
       </c>
       <c r="C26" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="D26" s="23" t="s">
-        <v>113</v>
-      </c>
       <c r="E26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -6345,13 +6162,13 @@
         <v>7</v>
       </c>
       <c r="C27" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="23" t="s">
-        <v>115</v>
-      </c>
       <c r="E27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -6362,13 +6179,13 @@
         <v>7</v>
       </c>
       <c r="C28" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D28" s="23" t="s">
-        <v>117</v>
-      </c>
       <c r="E28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -6379,13 +6196,13 @@
         <v>7</v>
       </c>
       <c r="C29" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>119</v>
-      </c>
       <c r="E29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -6396,13 +6213,13 @@
         <v>8</v>
       </c>
       <c r="C30" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="23" t="s">
-        <v>121</v>
-      </c>
       <c r="E30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -6413,13 +6230,13 @@
         <v>8</v>
       </c>
       <c r="C31" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>123</v>
-      </c>
       <c r="E31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -6430,13 +6247,13 @@
         <v>8</v>
       </c>
       <c r="C32" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="D32" s="23" t="s">
-        <v>125</v>
-      </c>
       <c r="E32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -6447,13 +6264,13 @@
         <v>8</v>
       </c>
       <c r="C33" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="D33" s="23" t="s">
-        <v>127</v>
-      </c>
       <c r="E33" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -6464,13 +6281,13 @@
         <v>9</v>
       </c>
       <c r="C34" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D34" s="23" t="s">
-        <v>129</v>
-      </c>
       <c r="E34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -6481,13 +6298,13 @@
         <v>9</v>
       </c>
       <c r="C35" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="D35" s="23" t="s">
-        <v>131</v>
-      </c>
       <c r="E35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -6498,13 +6315,13 @@
         <v>9</v>
       </c>
       <c r="C36" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="D36" s="23" t="s">
-        <v>133</v>
-      </c>
       <c r="E36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -6515,13 +6332,13 @@
         <v>9</v>
       </c>
       <c r="C37" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D37" s="23" t="s">
-        <v>135</v>
-      </c>
       <c r="E37" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -6532,13 +6349,13 @@
         <v>10</v>
       </c>
       <c r="C38" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="D38" s="23" t="s">
-        <v>137</v>
-      </c>
       <c r="E38" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -6549,13 +6366,13 @@
         <v>10</v>
       </c>
       <c r="C39" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D39" s="23" t="s">
-        <v>139</v>
-      </c>
       <c r="E39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -6566,13 +6383,13 @@
         <v>10</v>
       </c>
       <c r="C40" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D40" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="D40" s="23" t="s">
-        <v>141</v>
-      </c>
       <c r="E40" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -6583,13 +6400,13 @@
         <v>10</v>
       </c>
       <c r="C41" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="D41" s="23" t="s">
-        <v>143</v>
-      </c>
       <c r="E41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -6600,13 +6417,13 @@
         <v>11</v>
       </c>
       <c r="C42" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="D42" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="D42" s="23" t="s">
-        <v>145</v>
-      </c>
       <c r="E42" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30">
@@ -6617,13 +6434,13 @@
         <v>11</v>
       </c>
       <c r="C43" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D43" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="D43" s="23" t="s">
-        <v>147</v>
-      </c>
       <c r="E43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30">
@@ -6634,13 +6451,13 @@
         <v>11</v>
       </c>
       <c r="C44" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D44" s="23" t="s">
-        <v>149</v>
-      </c>
       <c r="E44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -6651,13 +6468,13 @@
         <v>11</v>
       </c>
       <c r="C45" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="D45" s="23" t="s">
-        <v>151</v>
-      </c>
       <c r="E45" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -6668,13 +6485,13 @@
         <v>12</v>
       </c>
       <c r="C46" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D46" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="D46" s="23" t="s">
-        <v>153</v>
-      </c>
       <c r="E46" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -6685,13 +6502,13 @@
         <v>12</v>
       </c>
       <c r="C47" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="D47" s="23" t="s">
-        <v>155</v>
-      </c>
       <c r="E47" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -6702,13 +6519,13 @@
         <v>12</v>
       </c>
       <c r="C48" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="D48" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="D48" s="23" t="s">
-        <v>157</v>
-      </c>
       <c r="E48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -6719,13 +6536,13 @@
         <v>12</v>
       </c>
       <c r="C49" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D49" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="D49" s="23" t="s">
-        <v>159</v>
-      </c>
       <c r="E49" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -6736,13 +6553,13 @@
         <v>13</v>
       </c>
       <c r="C50" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D50" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="D50" s="23" t="s">
-        <v>161</v>
-      </c>
       <c r="E50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -6753,13 +6570,13 @@
         <v>13</v>
       </c>
       <c r="C51" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="D51" s="23" t="s">
-        <v>163</v>
-      </c>
       <c r="E51" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -6770,13 +6587,13 @@
         <v>13</v>
       </c>
       <c r="C52" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="D52" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="D52" s="23" t="s">
-        <v>165</v>
-      </c>
       <c r="E52" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -6787,13 +6604,13 @@
         <v>13</v>
       </c>
       <c r="C53" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="D53" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="D53" s="23" t="s">
-        <v>167</v>
-      </c>
       <c r="E53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -6808,7 +6625,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6864,7 +6681,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6924,7 +6741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7017,10 +6834,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
+        <v>260</v>
+      </c>
+      <c r="H2" t="s">
         <v>261</v>
-      </c>
-      <c r="H2" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -7031,10 +6848,10 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
+        <v>262</v>
+      </c>
+      <c r="H3" t="s">
         <v>263</v>
-      </c>
-      <c r="H3" t="s">
-        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -7049,7 +6866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>